<commit_message>
corrected planned table structure
</commit_message>
<xml_diff>
--- a/recipes table schema.xlsx
+++ b/recipes table schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvasq\Repositories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvasq\Repositories\Recipository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19578A11-629A-4852-B61C-898AD9691757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5209D03A-8C1B-4749-AEE3-15968B5537BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19740" yWindow="4050" windowWidth="18255" windowHeight="15435" xr2:uid="{93A3302C-BA04-4AE9-842A-8D7F7FEBCDBB}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="38370" windowHeight="10500" xr2:uid="{93A3302C-BA04-4AE9-842A-8D7F7FEBCDBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Backend Tables" sheetId="1" r:id="rId1"/>
@@ -515,7 +515,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,9 +528,10 @@
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
init file structure and code setup for the server to define scoped needs. Using typescript and babel.
</commit_message>
<xml_diff>
--- a/recipes table schema.xlsx
+++ b/recipes table schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvasq\Repositories\Recipository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5209D03A-8C1B-4749-AEE3-15968B5537BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0593FF49-6F2E-474D-88A1-CE4D432016D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="38370" windowHeight="10500" xr2:uid="{93A3302C-BA04-4AE9-842A-8D7F7FEBCDBB}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{93A3302C-BA04-4AE9-842A-8D7F7FEBCDBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Backend Tables" sheetId="1" r:id="rId1"/>

</xml_diff>